<commit_message>
Se agregó la descarga de la semana de entrenamiento en la gestión de alumnos, utilizando el patrón template. Se agrego funcionalidad de backup a la aplicación, permitiendo realizar resguardo y restauración. Se creó la vista del Form de tablero, donde se representarán distintas métricas.
</commit_message>
<xml_diff>
--- a/SIGSE.FormsUI/bin/Debug/rutina.xlsx
+++ b/SIGSE.FormsUI/bin/Debug/rutina.xlsx
@@ -6,7 +6,7 @@
   </bookViews>
   <sheets>
     <sheet name="Dia1" sheetId="1" r:id="rId1"/>
-    <sheet name="Dia2" sheetId="2" r:id="rId3"/>
+    <sheet name="Dia2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -33,16 +33,16 @@
     <t>Descanso</t>
   </si>
   <si>
-    <t>Push 1</t>
+    <t>Torso 1</t>
   </si>
   <si>
     <t>Push 2</t>
   </si>
   <si>
-    <t>Pull 1</t>
-  </si>
-  <si>
-    <t>Pull 2</t>
+    <t>Pierna 2</t>
+  </si>
+  <si>
+    <t>Torso 2</t>
   </si>
 </sst>
 </file>
@@ -99,7 +99,7 @@
   <sheetPr>
     <tabColor rgb="FF000000"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -158,7 +158,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="0">
         <v>5</v>
@@ -178,7 +178,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="0">
         <v>5</v>
@@ -198,18 +198,178 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0">
+        <v>5</v>
+      </c>
+      <c r="D5" s="0">
+        <v>5</v>
+      </c>
+      <c r="E5" s="0">
+        <v>5</v>
+      </c>
+      <c r="F5" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0">
+        <v>5</v>
+      </c>
+      <c r="E6" s="0">
+        <v>5</v>
+      </c>
+      <c r="F6" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0">
+        <v>5</v>
+      </c>
+      <c r="E7" s="0">
+        <v>5</v>
+      </c>
+      <c r="F7" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="0">
+        <v>5</v>
+      </c>
+      <c r="D8" s="0">
+        <v>5</v>
+      </c>
+      <c r="E8" s="0">
+        <v>5</v>
+      </c>
+      <c r="F8" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0">
+        <v>5</v>
+      </c>
+      <c r="D9" s="0">
+        <v>5</v>
+      </c>
+      <c r="E9" s="0">
+        <v>5</v>
+      </c>
+      <c r="F9" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
-      <c r="C5" s="0">
-        <v>5</v>
-      </c>
-      <c r="D5" s="0">
-        <v>5</v>
-      </c>
-      <c r="E5" s="0">
-        <v>5</v>
-      </c>
-      <c r="F5" s="0">
+      <c r="B10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="0">
+        <v>5</v>
+      </c>
+      <c r="D10" s="0">
+        <v>5</v>
+      </c>
+      <c r="E10" s="0">
+        <v>5</v>
+      </c>
+      <c r="F10" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="0">
+        <v>5</v>
+      </c>
+      <c r="D11" s="0">
+        <v>5</v>
+      </c>
+      <c r="E11" s="0">
+        <v>5</v>
+      </c>
+      <c r="F11" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="0">
+        <v>5</v>
+      </c>
+      <c r="D12" s="0">
+        <v>5</v>
+      </c>
+      <c r="E12" s="0">
+        <v>5</v>
+      </c>
+      <c r="F12" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="0">
+        <v>5</v>
+      </c>
+      <c r="D13" s="0">
+        <v>5</v>
+      </c>
+      <c r="E13" s="0">
+        <v>5</v>
+      </c>
+      <c r="F13" s="0">
         <v>5</v>
       </c>
     </row>
@@ -223,7 +383,7 @@
   <sheetPr>
     <tabColor rgb="FF000000"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -262,7 +422,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0">
         <v>5</v>
@@ -282,7 +442,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0">
         <v>5</v>
@@ -302,7 +462,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="0">
         <v>5</v>
@@ -322,18 +482,98 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0">
+        <v>5</v>
+      </c>
+      <c r="D5" s="0">
+        <v>5</v>
+      </c>
+      <c r="E5" s="0">
+        <v>5</v>
+      </c>
+      <c r="F5" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="0">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0">
+        <v>5</v>
+      </c>
+      <c r="E6" s="0">
+        <v>5</v>
+      </c>
+      <c r="F6" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0">
+        <v>5</v>
+      </c>
+      <c r="E7" s="0">
+        <v>5</v>
+      </c>
+      <c r="F7" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0">
+        <v>5</v>
+      </c>
+      <c r="D8" s="0">
+        <v>5</v>
+      </c>
+      <c r="E8" s="0">
+        <v>5</v>
+      </c>
+      <c r="F8" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="0">
-        <v>5</v>
-      </c>
-      <c r="D5" s="0">
-        <v>5</v>
-      </c>
-      <c r="E5" s="0">
-        <v>5</v>
-      </c>
-      <c r="F5" s="0">
+      <c r="C9" s="0">
+        <v>5</v>
+      </c>
+      <c r="D9" s="0">
+        <v>5</v>
+      </c>
+      <c r="E9" s="0">
+        <v>5</v>
+      </c>
+      <c r="F9" s="0">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalización, tablero y modificación de entidades.
</commit_message>
<xml_diff>
--- a/SIGSE.FormsUI/bin/Debug/rutina.xlsx
+++ b/SIGSE.FormsUI/bin/Debug/rutina.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>#</t>
   </si>
@@ -33,16 +33,22 @@
     <t>Descanso</t>
   </si>
   <si>
-    <t>Torso 1</t>
-  </si>
-  <si>
-    <t>Push 2</t>
-  </si>
-  <si>
-    <t>Pierna 2</t>
-  </si>
-  <si>
-    <t>Torso 2</t>
+    <t>Ejercicio 1</t>
+  </si>
+  <si>
+    <t>Ejercicio 2</t>
+  </si>
+  <si>
+    <t>Ejercicio 4</t>
+  </si>
+  <si>
+    <t>Ejercicio 6</t>
+  </si>
+  <si>
+    <t>Ejercicio 12</t>
+  </si>
+  <si>
+    <t>Ejercicio 8</t>
   </si>
 </sst>
 </file>
@@ -99,14 +105,14 @@
   <sheetPr>
     <tabColor rgb="FF000000"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.7234289986747" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="12.2222202845982" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
@@ -158,7 +164,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0">
         <v>5</v>
@@ -178,7 +184,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0">
         <v>5</v>
@@ -198,7 +204,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0">
         <v>5</v>
@@ -218,7 +224,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0">
         <v>5</v>
@@ -238,7 +244,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0">
         <v>5</v>
@@ -250,126 +256,6 @@
         <v>5</v>
       </c>
       <c r="F7" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="0">
-        <v>5</v>
-      </c>
-      <c r="D8" s="0">
-        <v>5</v>
-      </c>
-      <c r="E8" s="0">
-        <v>5</v>
-      </c>
-      <c r="F8" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="0">
-        <v>5</v>
-      </c>
-      <c r="D9" s="0">
-        <v>5</v>
-      </c>
-      <c r="E9" s="0">
-        <v>5</v>
-      </c>
-      <c r="F9" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="0">
-        <v>5</v>
-      </c>
-      <c r="D10" s="0">
-        <v>5</v>
-      </c>
-      <c r="E10" s="0">
-        <v>5</v>
-      </c>
-      <c r="F10" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="0">
-        <v>5</v>
-      </c>
-      <c r="D11" s="0">
-        <v>5</v>
-      </c>
-      <c r="E11" s="0">
-        <v>5</v>
-      </c>
-      <c r="F11" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0">
-        <v>11</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="0">
-        <v>5</v>
-      </c>
-      <c r="D12" s="0">
-        <v>5</v>
-      </c>
-      <c r="E12" s="0">
-        <v>5</v>
-      </c>
-      <c r="F12" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0">
-        <v>12</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="0">
-        <v>5</v>
-      </c>
-      <c r="D13" s="0">
-        <v>5</v>
-      </c>
-      <c r="E13" s="0">
-        <v>5</v>
-      </c>
-      <c r="F13" s="0">
         <v>5</v>
       </c>
     </row>
@@ -383,14 +269,14 @@
   <sheetPr>
     <tabColor rgb="FF000000"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.62977273123605" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="12.2222202845982" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
@@ -422,7 +308,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0">
         <v>5</v>
@@ -442,7 +328,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0">
         <v>5</v>
@@ -462,7 +348,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0">
         <v>5</v>
@@ -482,7 +368,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0">
         <v>5</v>
@@ -494,86 +380,6 @@
         <v>5</v>
       </c>
       <c r="F5" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="0">
-        <v>5</v>
-      </c>
-      <c r="D6" s="0">
-        <v>5</v>
-      </c>
-      <c r="E6" s="0">
-        <v>5</v>
-      </c>
-      <c r="F6" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="0">
-        <v>5</v>
-      </c>
-      <c r="D7" s="0">
-        <v>5</v>
-      </c>
-      <c r="E7" s="0">
-        <v>5</v>
-      </c>
-      <c r="F7" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="0">
-        <v>5</v>
-      </c>
-      <c r="D8" s="0">
-        <v>5</v>
-      </c>
-      <c r="E8" s="0">
-        <v>5</v>
-      </c>
-      <c r="F8" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="0">
-        <v>5</v>
-      </c>
-      <c r="D9" s="0">
-        <v>5</v>
-      </c>
-      <c r="E9" s="0">
-        <v>5</v>
-      </c>
-      <c r="F9" s="0">
         <v>5</v>
       </c>
     </row>

</xml_diff>